<commit_message>
Add the result of LDA-T4 from server
</commit_message>
<xml_diff>
--- a/output/LDA-T4-result.xlsx
+++ b/output/LDA-T4-result.xlsx
@@ -8,13 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="LDA_5" sheetId="1" r:id="rId1"/>
+    <sheet name="LDA_10" sheetId="2" r:id="rId2"/>
+    <sheet name="LDA_15" sheetId="3" r:id="rId3"/>
+    <sheet name="LDA_25" sheetId="4" r:id="rId4"/>
+    <sheet name="LDA_50" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="5">
   <si>
     <t>train</t>
   </si>
@@ -532,4 +536,604 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>400</v>
+      </c>
+      <c r="D2">
+        <v>0.6325878594249201</v>
+      </c>
+      <c r="E2">
+        <v>0.5038167938931297</v>
+      </c>
+      <c r="F2">
+        <v>0.5609065155807366</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3">
+        <v>500</v>
+      </c>
+      <c r="D3">
+        <v>0.7467532467532467</v>
+      </c>
+      <c r="E3">
+        <v>0.5852417302798982</v>
+      </c>
+      <c r="F3">
+        <v>0.6562054208273894</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>400</v>
+      </c>
+      <c r="C4">
+        <v>600</v>
+      </c>
+      <c r="D4">
+        <v>0.8307210031347962</v>
+      </c>
+      <c r="E4">
+        <v>0.6743002544529262</v>
+      </c>
+      <c r="F4">
+        <v>0.7443820224719101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>600</v>
+      </c>
+      <c r="C5">
+        <v>600</v>
+      </c>
+      <c r="D5">
+        <v>0.8442367601246106</v>
+      </c>
+      <c r="E5">
+        <v>0.6895674300254453</v>
+      </c>
+      <c r="F5">
+        <v>0.7591036414565826</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6">
+        <v>600</v>
+      </c>
+      <c r="D6">
+        <v>0.8363095238095238</v>
+      </c>
+      <c r="E6">
+        <v>0.7150127226463104</v>
+      </c>
+      <c r="F6">
+        <v>0.7709190672153636</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1200</v>
+      </c>
+      <c r="C7">
+        <v>600</v>
+      </c>
+      <c r="D7">
+        <v>0.831858407079646</v>
+      </c>
+      <c r="E7">
+        <v>0.7175572519083969</v>
+      </c>
+      <c r="F7">
+        <v>0.7704918032786884</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>400</v>
+      </c>
+      <c r="D2">
+        <v>0.6293929712460063</v>
+      </c>
+      <c r="E2">
+        <v>0.5012722646310432</v>
+      </c>
+      <c r="F2">
+        <v>0.5580736543909349</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3">
+        <v>500</v>
+      </c>
+      <c r="D3">
+        <v>0.737012987012987</v>
+      </c>
+      <c r="E3">
+        <v>0.5776081424936387</v>
+      </c>
+      <c r="F3">
+        <v>0.6476462196861626</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>400</v>
+      </c>
+      <c r="C4">
+        <v>600</v>
+      </c>
+      <c r="D4">
+        <v>0.8401253918495298</v>
+      </c>
+      <c r="E4">
+        <v>0.6819338422391857</v>
+      </c>
+      <c r="F4">
+        <v>0.7528089887640449</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>600</v>
+      </c>
+      <c r="C5">
+        <v>600</v>
+      </c>
+      <c r="D5">
+        <v>0.84472049689441</v>
+      </c>
+      <c r="E5">
+        <v>0.6921119592875318</v>
+      </c>
+      <c r="F5">
+        <v>0.7608391608391609</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6">
+        <v>600</v>
+      </c>
+      <c r="D6">
+        <v>0.8422619047619048</v>
+      </c>
+      <c r="E6">
+        <v>0.7201017811704835</v>
+      </c>
+      <c r="F6">
+        <v>0.776406035665295</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1200</v>
+      </c>
+      <c r="C7">
+        <v>600</v>
+      </c>
+      <c r="D7">
+        <v>0.8323529411764706</v>
+      </c>
+      <c r="E7">
+        <v>0.7201017811704835</v>
+      </c>
+      <c r="F7">
+        <v>0.7721691678035471</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>400</v>
+      </c>
+      <c r="D2">
+        <v>0.6217948717948718</v>
+      </c>
+      <c r="E2">
+        <v>0.4936386768447837</v>
+      </c>
+      <c r="F2">
+        <v>0.550354609929078</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3">
+        <v>500</v>
+      </c>
+      <c r="D3">
+        <v>0.737012987012987</v>
+      </c>
+      <c r="E3">
+        <v>0.5776081424936387</v>
+      </c>
+      <c r="F3">
+        <v>0.6476462196861626</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>400</v>
+      </c>
+      <c r="C4">
+        <v>600</v>
+      </c>
+      <c r="D4">
+        <v>0.8401253918495298</v>
+      </c>
+      <c r="E4">
+        <v>0.6819338422391857</v>
+      </c>
+      <c r="F4">
+        <v>0.7528089887640449</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>600</v>
+      </c>
+      <c r="C5">
+        <v>600</v>
+      </c>
+      <c r="D5">
+        <v>0.8478260869565217</v>
+      </c>
+      <c r="E5">
+        <v>0.6946564885496184</v>
+      </c>
+      <c r="F5">
+        <v>0.7636363636363636</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6">
+        <v>600</v>
+      </c>
+      <c r="D6">
+        <v>0.8482142857142857</v>
+      </c>
+      <c r="E6">
+        <v>0.7251908396946565</v>
+      </c>
+      <c r="F6">
+        <v>0.7818930041152264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1200</v>
+      </c>
+      <c r="C7">
+        <v>600</v>
+      </c>
+      <c r="D7">
+        <v>0.8382352941176471</v>
+      </c>
+      <c r="E7">
+        <v>0.7251908396946565</v>
+      </c>
+      <c r="F7">
+        <v>0.7776261937244201</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>400</v>
+      </c>
+      <c r="D2">
+        <v>0.6217948717948718</v>
+      </c>
+      <c r="E2">
+        <v>0.4936386768447837</v>
+      </c>
+      <c r="F2">
+        <v>0.550354609929078</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3">
+        <v>500</v>
+      </c>
+      <c r="D3">
+        <v>0.737012987012987</v>
+      </c>
+      <c r="E3">
+        <v>0.5776081424936387</v>
+      </c>
+      <c r="F3">
+        <v>0.6476462196861626</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>400</v>
+      </c>
+      <c r="C4">
+        <v>600</v>
+      </c>
+      <c r="D4">
+        <v>0.8401253918495298</v>
+      </c>
+      <c r="E4">
+        <v>0.6819338422391857</v>
+      </c>
+      <c r="F4">
+        <v>0.7528089887640449</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>600</v>
+      </c>
+      <c r="C5">
+        <v>600</v>
+      </c>
+      <c r="D5">
+        <v>0.84472049689441</v>
+      </c>
+      <c r="E5">
+        <v>0.6921119592875318</v>
+      </c>
+      <c r="F5">
+        <v>0.7608391608391609</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6">
+        <v>600</v>
+      </c>
+      <c r="D6">
+        <v>0.8482142857142857</v>
+      </c>
+      <c r="E6">
+        <v>0.7251908396946565</v>
+      </c>
+      <c r="F6">
+        <v>0.7818930041152264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1200</v>
+      </c>
+      <c r="C7">
+        <v>600</v>
+      </c>
+      <c r="D7">
+        <v>0.8382352941176471</v>
+      </c>
+      <c r="E7">
+        <v>0.7251908396946565</v>
+      </c>
+      <c r="F7">
+        <v>0.7776261937244201</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>